<commit_message>
fix bugs / update core runner / add index interface
</commit_message>
<xml_diff>
--- a/docs/接口文档.xlsx
+++ b/docs/接口文档.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{03DE396B-9110-4E09-BEAF-FDBFE64670C3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="项目管理" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="75">
   <si>
     <t xml:space="preserve">    {
         "productid":"5",
@@ -327,11 +328,18 @@
     <t>这个接口是给新增用例等东西的时候，选择所属模块用的</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>runtests</t>
+  </si>
+  <si>
+    <t>执行用例</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -453,7 +461,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -528,6 +536,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -563,6 +588,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -738,11 +780,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F20" activeCellId="1" sqref="F19 F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1100,35 +1142,53 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20" s="7"/>
       <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="7"/>
+      <c r="B21" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="F21" s="6" t="s">
-        <v>61</v>
+      <c r="F21" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="F22" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F23" s="6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1136,10 +1196,10 @@
   <mergeCells count="3">
     <mergeCell ref="A2:A8"/>
     <mergeCell ref="A9:A15"/>
-    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A16:A21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug and add reporter managements
</commit_message>
<xml_diff>
--- a/docs/接口文档.xlsx
+++ b/docs/接口文档.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A0B3FB8F-E06A-4141-9A2B-FB4597D5B6CA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{59D874A4-814E-4E85-9309-BDB51F1AC5F0}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
   <si>
     <t>更新产品信息</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -206,10 +206,6 @@
   </si>
   <si>
     <t>报告管理</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>需要改级联删除功能</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1532,6 +1528,154 @@
     <t>/runproduct</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>获取根据版本获取用例执行结果（默认为最后一次）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>post</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/getreports</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    {"version":""}：默认最后一次
+    {"version":5}：版本为5的报告</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": 200,
+    "data": [
+        {
+            "cassid": 1,
+            "createtime": "2018-05-18 14:33:09",
+            "id": 69,
+            "result": "",
+            "runtime": "",
+            "status": "报错",
+            "validate": "",
+            "version": 14
+        },
+        {
+            "cassid": 2,
+            "createtime": "2018-05-18 14:33:10",
+            "id": 70,
+            "result": "",
+            "runtime": "",
+            "status": "报错",
+            "validate": "",
+            "version": 14
+        },
+        {
+            "cassid": 3,
+            "createtime": "2018-05-18 14:33:10",
+            "id": 71,
+            "result": "",
+            "runtime": "",
+            "status": "报错",
+            "validate": "",
+            "version": 14
+        }
+    ],
+    "msg": "查询成功！！！"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取所有执行版本</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/getversions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": 200,
+    "data": {
+        "versions": [
+            1,
+            2,
+            3,
+            4,
+            5,
+            6,
+            7,
+            8,
+            9,
+            10,
+            11,
+            12,
+            13,
+            14
+        ]
+    },
+    "msg": "查询成功！！！"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>条件查询测试结果饼图</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/conditionquerytestress</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据不同的条件进行查询，参数可以传以下内容
+{} 
+{"version": 14} 
+{"version": 14, "productid": 1}
+{"version": 14, "productid": 1, "projectid": 1} 
+{"version": 14, "productid": 1, "projectid": 1, "moduleid": 6}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "code": 200,
+    "data": {
+        "failed": {
+            "count": 2,
+            "data": [
+                {
+                    "cassid": 2,
+                    "createtime": "2018-05-18 14:33:10",
+                    "id": 70,
+                    "result": "",
+                    "runtime": "",
+                    "status": "报错",
+                    "validate": "",
+                    "version": 14
+                },
+                {
+                    "cassid": 3,
+                    "createtime": "2018-05-18 14:33:10",
+                    "id": 71,
+                    "result": "",
+                    "runtime": "",
+                    "status": "报错",
+                    "validate": "",
+                    "version": 14
+                }
+            ]
+        },
+        "success": {
+            "count": 0,
+            "data": []
+        }
+    },
+    "msg": "查询成功!"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1628,10 +1772,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1971,10 +2115,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2008,14 +2152,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>113</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>21</v>
@@ -2024,50 +2168,50 @@
         <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="6" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="8"/>
+      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="7"/>
-      <c r="B4" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2075,35 +2219,33 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="7"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>42</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="7"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
@@ -2117,11 +2259,11 @@
         <v>5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="108" x14ac:dyDescent="0.15">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
@@ -2135,16 +2277,16 @@
         <v>13</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.15">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>21</v>
@@ -2153,11 +2295,11 @@
         <v>14</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2173,63 +2315,63 @@
         <v>25</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A13" s="8"/>
+      <c r="B13" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A13" s="7"/>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="7"/>
+      <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
@@ -2240,14 +2382,14 @@
         <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="15" spans="1:7" ht="108" x14ac:dyDescent="0.15">
-      <c r="A15" s="7"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
@@ -2261,29 +2403,29 @@
         <v>30</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.15">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="147.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="8" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -2293,196 +2435,274 @@
         <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A18" s="7"/>
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A19" s="7"/>
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>83</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>23</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A20" s="7"/>
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.15">
+      <c r="A21" s="8"/>
+      <c r="B21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.15">
-      <c r="A21" s="7"/>
-      <c r="B21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>91</v>
-      </c>
     </row>
     <row r="22" spans="1:7" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="6" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A23" s="7" t="s">
+      <c r="C23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="8"/>
+      <c r="B24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A25" s="8"/>
+      <c r="B25" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A26" s="8"/>
+      <c r="B26" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A27" s="8"/>
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D27" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A24" s="7"/>
-      <c r="B24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A25" s="7"/>
-      <c r="B25" s="2" t="s">
+      <c r="F27" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A28" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A26" s="7"/>
-      <c r="B26" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="2" t="s">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A29" s="8"/>
+      <c r="B29" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A27" s="7"/>
-      <c r="B27" s="2" t="s">
+      <c r="C29" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A28" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A30" s="7"/>
+    </row>
+    <row r="30" spans="1:7" ht="22.5" x14ac:dyDescent="0.15">
+      <c r="A30" s="8"/>
+      <c r="B30" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A32" s="7"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A32" s="8"/>
+      <c r="B32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A33" s="8"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2490,7 +2710,7 @@
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A28:A36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix bug and add configs module
</commit_message>
<xml_diff>
--- a/docs/接口文档.xlsx
+++ b/docs/接口文档.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EFB52DD8-A315-40A2-A2A6-83D343D0366C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="项目管理" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="136">
   <si>
     <t>更新产品信息</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1710,11 +1709,40 @@
     <t>/conditionqueryreports</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>公共配置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>导入测试用例</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>/uploadtestcase</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>参见uploadDemo.html</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>上传文件:
+1. examples/har_test.har
+2. eamples/postman_test.json</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+  "code": 200, 
+  "msg": "执行成功,成功导入2个,失败0个"
+}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1787,7 +1815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1811,6 +1839,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1829,7 +1860,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1904,23 +1935,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1956,23 +1970,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2148,11 +2145,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2744,14 +2741,31 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A34" s="8"/>
+    <row r="34" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+      <c r="A34" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A35" s="8"/>
+      <c r="A35" s="9"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A36" s="8"/>
+      <c r="A36" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2759,7 +2773,7 @@
     <mergeCell ref="A10:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A23:A27"/>
-    <mergeCell ref="A28:A36"/>
+    <mergeCell ref="A28:A33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>